<commit_message>
Add many algorithm tests and flag to skip input validation (Issue #17)
</commit_message>
<xml_diff>
--- a/test_data/by_matching/p_same_first_choice.xlsx
+++ b/test_data/by_matching/p_same_first_choice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferestigene/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lonnychen/Dropbox/@project - HERTIE SCHOOL/MDS/COURSES/Spring 2024/Data Structures &amp; Algorithms (C9)/Project/student-project-matching/test_data/by_matching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655B01D7-F4F3-A941-8449-FBBAC5733D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71E71FA-135A-0943-B06A-971E84BC7BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14360" yWindow="500" windowWidth="14440" windowHeight="15300" xr2:uid="{B15B0C67-31C5-7345-86DF-5081700ECC51}"/>
   </bookViews>
@@ -80,13 +80,13 @@
     <t>3rd_choice</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
   </si>
 </sst>
 </file>
@@ -190,9 +190,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -230,7 +230,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -336,7 +336,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -478,7 +478,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>